<commit_message>
with box stacking problem
</commit_message>
<xml_diff>
--- a/Questions_to_solve.xlsx
+++ b/Questions_to_solve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allwin\Documents\Important-Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C128AB-724F-43E7-9DCB-1473AF534164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92393116-04CC-4CEA-8ADE-8F488CCF6CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{9ECBBF44-6BC2-DF4A-90F0-7712912C1734}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
   <si>
     <t>Easy</t>
   </si>
@@ -325,6 +325,15 @@
   </si>
   <si>
     <t>Q/day</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Target</t>
   </si>
 </sst>
 </file>
@@ -895,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51E3EE9-A70D-A94A-9E6D-6F3030F6E9C5}">
   <dimension ref="B1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1010,7 +1019,7 @@
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="21" t="s">
         <v>43</v>
       </c>
       <c r="O4" s="1"/>
@@ -1037,7 +1046,7 @@
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="21" t="s">
         <v>44</v>
       </c>
       <c r="O5" s="1"/>
@@ -1064,7 +1073,7 @@
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="21" t="s">
         <v>45</v>
       </c>
       <c r="O6" s="1"/>
@@ -1086,12 +1095,12 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="21" t="s">
         <v>33</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="21" t="s">
         <v>46</v>
       </c>
       <c r="O7" s="1"/>
@@ -1109,12 +1118,12 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="21" t="s">
         <v>34</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="21" t="s">
         <v>47</v>
       </c>
       <c r="O8" s="1"/>
@@ -1146,12 +1155,12 @@
         <f>4*G9</f>
         <v>16</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="21" t="s">
         <v>35</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="21" t="s">
         <v>48</v>
       </c>
       <c r="O9" s="1"/>
@@ -1173,12 +1182,12 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="21" t="s">
         <v>36</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="N10" s="3" t="s">
+      <c r="N10" s="21" t="s">
         <v>49</v>
       </c>
       <c r="O10" s="1"/>
@@ -1198,12 +1207,12 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="21" t="s">
         <v>37</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="N11" s="3" t="s">
+      <c r="N11" s="21" t="s">
         <v>50</v>
       </c>
       <c r="O11" s="1"/>
@@ -1230,12 +1239,12 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="21" t="s">
         <v>38</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="N12" s="3" t="s">
+      <c r="N12" s="21" t="s">
         <v>51</v>
       </c>
       <c r="O12" s="1"/>
@@ -1257,7 +1266,7 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="21" t="s">
         <v>39</v>
       </c>
       <c r="K13" s="1"/>
@@ -1274,7 +1283,7 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="21" t="s">
         <v>40</v>
       </c>
       <c r="K14" s="1"/>
@@ -1291,7 +1300,7 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="21" t="s">
         <v>41</v>
       </c>
       <c r="K15" s="1"/>
@@ -1569,7 +1578,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>82</v>
       </c>
@@ -1580,8 +1589,15 @@
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>100</v>
+      </c>
+      <c r="L33">
+        <f>D3+D12+H3+H9+L3+4</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>83</v>
       </c>
@@ -1592,8 +1608,19 @@
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>101</v>
+      </c>
+      <c r="M34">
+        <f>M32-L33-24</f>
+        <v>156</v>
+      </c>
+      <c r="N34">
+        <f>M34/16</f>
+        <v>9.75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1602,13 +1629,20 @@
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L35" t="s">
+        <v>102</v>
+      </c>
+      <c r="M35">
+        <f>M34/20</f>
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F37" s="2" t="s">
         <v>92</v>
       </c>
@@ -1620,21 +1654,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F38" s="3" t="s">
         <v>75</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F39" s="3" t="s">
         <v>93</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F40" s="3" t="s">
         <v>94</v>
       </c>

</xml_diff>